<commit_message>
Finish Practicing I/S Sort
</commit_message>
<xml_diff>
--- a/Past Exams/midterm3/Selection-Insertion Sort Practice.xlsx
+++ b/Past Exams/midterm3/Selection-Insertion Sort Practice.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbry1\OneDrive\Documents\CS1324\Past Exams\midterm3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E0EC8494-4C62-4CFA-89DD-801636AA859D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B977A948-C141-4B66-AABA-F863372BAE52}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{804A91AC-DC47-4070-91D5-379C2068E1BA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Comparative" sheetId="2" r:id="rId1"/>
+    <sheet name="Insertion 1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029" iterate="1" calcOnSave="0"/>
   <extLst>
@@ -31,9 +32,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
   <si>
     <t>Aux</t>
+  </si>
+  <si>
+    <t>Selection Sort</t>
+  </si>
+  <si>
+    <t>Insertion Sort</t>
   </si>
 </sst>
 </file>
@@ -43,7 +50,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_(* #,##0_);[Red]_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -62,12 +69,20 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -85,8 +100,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -114,8 +135,37 @@
       <right/>
       <top/>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
         <color theme="4" tint="0.39991454817346722"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -151,6 +201,79 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39991454817346722"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39991454817346722"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -162,16 +285,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,12 +646,357 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6CDE2D5-3901-4B8B-A620-9226C6481DF2}">
-  <dimension ref="B2:L46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1BC19CA-937A-4693-90C3-3A64F78AF0DC}">
+  <dimension ref="B2:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L16" sqref="L16"/>
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="7" max="8" width="2.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B2" s="5">
+        <f>MIN(B6:B17)</f>
+        <v>18</v>
+      </c>
+      <c r="C2" s="5">
+        <f>MIN(C6:C17)</f>
+        <v>23</v>
+      </c>
+      <c r="D2" s="5">
+        <f>MIN(D6:D17)</f>
+        <v>38</v>
+      </c>
+      <c r="E2" s="5">
+        <f>MIN(E6:E17)</f>
+        <v>52</v>
+      </c>
+      <c r="F2" s="5">
+        <f>MIN(F6:F17)</f>
+        <v>78</v>
+      </c>
+      <c r="I2" s="5">
+        <f>MIN(I6:I17)</f>
+        <v>18</v>
+      </c>
+      <c r="J2" s="5">
+        <f>MIN(J6:J17)</f>
+        <v>23</v>
+      </c>
+      <c r="K2" s="5">
+        <f>MIN(K6:K17)</f>
+        <v>38</v>
+      </c>
+      <c r="L2" s="5">
+        <f>MIN(L6:L17)</f>
+        <v>52</v>
+      </c>
+      <c r="M2" s="5">
+        <f>MIN(M6:M17)</f>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="10"/>
+      <c r="I4" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="21"/>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="11">
+        <v>38</v>
+      </c>
+      <c r="C5" s="1">
+        <v>78</v>
+      </c>
+      <c r="D5" s="1">
+        <v>18</v>
+      </c>
+      <c r="E5" s="1">
+        <v>23</v>
+      </c>
+      <c r="F5" s="12">
+        <v>52</v>
+      </c>
+      <c r="I5" s="11">
+        <f>B5</f>
+        <v>38</v>
+      </c>
+      <c r="J5" s="1">
+        <f t="shared" ref="J5:O5" si="0">C5</f>
+        <v>78</v>
+      </c>
+      <c r="K5" s="1">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="L5" s="1">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="M5" s="1">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="13">
+        <f>D5</f>
+        <v>18</v>
+      </c>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14">
+        <f>B5</f>
+        <v>38</v>
+      </c>
+      <c r="E6" s="14"/>
+      <c r="F6" s="15"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="3">
+        <f>J5</f>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B7" s="13"/>
+      <c r="C7" s="14">
+        <f>E5</f>
+        <v>23</v>
+      </c>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14">
+        <f>C5</f>
+        <v>78</v>
+      </c>
+      <c r="F7" s="15"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14">
+        <f>J5</f>
+        <v>78</v>
+      </c>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+      <c r="N7" s="3"/>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="13"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14">
+        <f>B5</f>
+        <v>38</v>
+      </c>
+      <c r="E8" s="14"/>
+      <c r="F8" s="15"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="14">
+        <f>I5</f>
+        <v>38</v>
+      </c>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="3"/>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B9" s="13"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14">
+        <f>F5</f>
+        <v>52</v>
+      </c>
+      <c r="F9" s="15">
+        <f>E7</f>
+        <v>78</v>
+      </c>
+      <c r="I9" s="13">
+        <f>K5</f>
+        <v>18</v>
+      </c>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="3"/>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B10" s="13"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="15">
+        <f>F9</f>
+        <v>78</v>
+      </c>
+      <c r="I10" s="13"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="3">
+        <f>L5</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B11" s="13"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="15"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14">
+        <f>K7</f>
+        <v>78</v>
+      </c>
+      <c r="M11" s="14"/>
+      <c r="N11" s="3"/>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B12" s="13"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="15"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14">
+        <f>J8</f>
+        <v>38</v>
+      </c>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="3"/>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B13" s="13"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="15"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="14">
+        <f>N10</f>
+        <v>23</v>
+      </c>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="3"/>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B14" s="13"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="15"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+      <c r="N14" s="3">
+        <f>M5</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B15" s="13"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="15"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="14">
+        <f>L11</f>
+        <v>78</v>
+      </c>
+      <c r="N15" s="3"/>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B16" s="13"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="15"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="14">
+        <f>N14</f>
+        <v>52</v>
+      </c>
+      <c r="M16" s="14"/>
+      <c r="N16" s="3"/>
+    </row>
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B17" s="13"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="15"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+      <c r="N17" s="3"/>
+    </row>
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B18" s="16"/>
+      <c r="C18" s="17"/>
+      <c r="D18" s="17"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="18"/>
+      <c r="I18" s="16"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6CDE2D5-3901-4B8B-A620-9226C6481DF2}">
+  <dimension ref="B2:L47"/>
+  <sheetViews>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,340 +1006,355 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="1">
+      <c r="B2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B3" s="1">
         <v>51</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C3" s="1">
         <v>83</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D3" s="1">
         <v>92</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E3" s="1">
         <v>3</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F3" s="1">
         <v>22</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G3" s="1">
         <v>98</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H3" s="1">
         <v>72</v>
       </c>
-      <c r="I2" s="1">
+      <c r="I3" s="1">
         <v>24</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J3" s="1">
         <v>16</v>
       </c>
-      <c r="K2" s="1">
+      <c r="K3" s="1">
         <v>1</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="L3" s="3">
-        <f>E2</f>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L4" s="3">
+        <f>E3</f>
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E4">
-        <f>D2</f>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <f>D3</f>
         <v>92</v>
       </c>
-      <c r="L4" s="3"/>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D5">
-        <f>C2</f>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <f>C3</f>
         <v>83</v>
       </c>
-      <c r="L5" s="3"/>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C6">
-        <f>B2</f>
+      <c r="L6" s="3"/>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <f>B3</f>
         <v>51</v>
       </c>
-      <c r="L6" s="3"/>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7">
-        <f>E2</f>
+      <c r="L7" s="3"/>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <f>E3</f>
         <v>3</v>
       </c>
-      <c r="L7" s="3"/>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="L8" s="3">
-        <f>F2</f>
+      <c r="L8" s="3"/>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L9" s="3">
+        <f>F3</f>
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F9">
-        <f>E4</f>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <f>E5</f>
         <v>92</v>
       </c>
-      <c r="L9" s="3"/>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E10">
-        <f>D5</f>
+      <c r="L10" s="3"/>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <f>D6</f>
         <v>83</v>
       </c>
-      <c r="L10" s="3"/>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D11">
-        <f>C6</f>
+      <c r="L11" s="3"/>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <f>C7</f>
         <v>51</v>
       </c>
-      <c r="L11" s="3"/>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C12">
-        <f>L8</f>
+      <c r="L12" s="3"/>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <f>L9</f>
         <v>22</v>
       </c>
-      <c r="L12" s="3"/>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="L13" s="3">
-        <f>G2</f>
+      <c r="L13" s="3"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L14" s="3">
+        <f>G3</f>
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="G14">
-        <f>G2</f>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <f>G3</f>
         <v>98</v>
       </c>
-      <c r="L14" s="3"/>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="L15" s="3">
-        <f>H2</f>
+      <c r="L15" s="3"/>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L16" s="3">
+        <f>H3</f>
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="H16">
-        <f>G14</f>
+    <row r="17" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <f>G15</f>
         <v>98</v>
       </c>
-      <c r="L16" s="3"/>
-    </row>
-    <row r="17" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="G17">
-        <f>F9</f>
+      <c r="L17" s="3"/>
+    </row>
+    <row r="18" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <f>F10</f>
         <v>92</v>
       </c>
-      <c r="L17" s="3"/>
-    </row>
-    <row r="18" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="F18">
-        <f>E10</f>
+      <c r="L18" s="3"/>
+    </row>
+    <row r="19" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <f>E11</f>
         <v>83</v>
       </c>
-      <c r="L18" s="3"/>
-    </row>
-    <row r="19" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="E19">
-        <f>L15</f>
+      <c r="L19" s="3"/>
+    </row>
+    <row r="20" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <f>L16</f>
         <v>72</v>
       </c>
-      <c r="L19" s="3"/>
-    </row>
-    <row r="20" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="L20" s="3">
-        <f>I2</f>
+      <c r="L20" s="3"/>
+    </row>
+    <row r="21" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="L21" s="3">
+        <f>I3</f>
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="I21">
-        <f>H16</f>
+    <row r="22" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="I22">
+        <f>H17</f>
         <v>98</v>
       </c>
-      <c r="L21" s="3"/>
-    </row>
-    <row r="22" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="H22">
-        <f>G17</f>
+      <c r="L22" s="3"/>
+    </row>
+    <row r="23" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="H23">
+        <f>G18</f>
         <v>92</v>
       </c>
-      <c r="L22" s="3"/>
-    </row>
-    <row r="23" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="G23">
-        <f>F18</f>
+      <c r="L23" s="3"/>
+    </row>
+    <row r="24" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="G24">
+        <f>F19</f>
         <v>83</v>
       </c>
-      <c r="L23" s="3"/>
-    </row>
-    <row r="24" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="F24">
-        <f>E19</f>
+      <c r="L24" s="3"/>
+    </row>
+    <row r="25" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <f>E20</f>
         <v>72</v>
       </c>
-      <c r="L24" s="3"/>
-    </row>
-    <row r="25" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="E25">
-        <f>D11</f>
+      <c r="L25" s="3"/>
+    </row>
+    <row r="26" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <f>D12</f>
         <v>51</v>
       </c>
-      <c r="L25" s="3"/>
-    </row>
-    <row r="26" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D26">
-        <f>L20</f>
+      <c r="L26" s="3"/>
+    </row>
+    <row r="27" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="D27">
+        <f>L21</f>
         <v>24</v>
       </c>
-      <c r="L26" s="3"/>
-    </row>
-    <row r="27" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="L27" s="3">
-        <f>J2</f>
+      <c r="L27" s="3"/>
+    </row>
+    <row r="28" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="L28" s="3">
+        <f>J3</f>
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="J28">
-        <f>MIN(I$3:I28)</f>
+    <row r="29" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="J29">
+        <f>MIN(I$4:I29)</f>
         <v>98</v>
       </c>
-      <c r="L28" s="3"/>
-    </row>
-    <row r="29" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="I29">
-        <f>MIN(H$3:H29)</f>
+      <c r="L29" s="3"/>
+    </row>
+    <row r="30" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="I30">
+        <f>MIN(H$4:H30)</f>
         <v>92</v>
       </c>
-      <c r="L29" s="3"/>
-    </row>
-    <row r="30" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="H30">
-        <f>MIN(G$3:G30)</f>
+      <c r="L30" s="3"/>
+    </row>
+    <row r="31" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="H31">
+        <f>MIN(G$4:G31)</f>
         <v>83</v>
       </c>
-      <c r="L30" s="3"/>
-    </row>
-    <row r="31" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="G31">
-        <f>MIN(F$3:F31)</f>
+      <c r="L31" s="3"/>
+    </row>
+    <row r="32" spans="4:12" x14ac:dyDescent="0.25">
+      <c r="G32">
+        <f>MIN(F$4:F32)</f>
         <v>72</v>
       </c>
-      <c r="L31" s="3"/>
-    </row>
-    <row r="32" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="F32">
-        <f>MIN(E$3:E32)</f>
+      <c r="L32" s="3"/>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <f>MIN(E$4:E33)</f>
         <v>51</v>
       </c>
-      <c r="L32" s="3"/>
-    </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E33">
-        <f>MIN(D$3:D33)</f>
+      <c r="L33" s="3"/>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <f>MIN(D$4:D34)</f>
         <v>24</v>
       </c>
-      <c r="L33" s="3"/>
-    </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D34">
-        <f>MIN(C$3:C34)</f>
+      <c r="L34" s="3"/>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <f>MIN(C$4:C35)</f>
         <v>22</v>
       </c>
-      <c r="L34" s="3"/>
-    </row>
-    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C35">
-        <f>L27</f>
+      <c r="L35" s="3"/>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <f>L28</f>
         <v>16</v>
       </c>
-      <c r="L35" s="3"/>
-    </row>
-    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="L36" s="3">
-        <f>K2</f>
+      <c r="L36" s="3"/>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="L37" s="3">
+        <f>K3</f>
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="K37">
-        <f>MIN(J$3:J37)</f>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="K38">
+        <f>MIN(J$4:J38)</f>
         <v>98</v>
       </c>
-      <c r="L37" s="3"/>
-    </row>
-    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="J38">
-        <f>MIN(I$3:I38)</f>
+      <c r="L38" s="3"/>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="J39">
+        <f>MIN(I$4:I39)</f>
         <v>92</v>
       </c>
-      <c r="L38" s="3"/>
-    </row>
-    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="I39">
-        <f>MIN(H$3:H39)</f>
+      <c r="L39" s="3"/>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="I40">
+        <f>MIN(H$4:H40)</f>
         <v>83</v>
       </c>
-      <c r="L39" s="3"/>
-    </row>
-    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="H40">
-        <f>MIN(G$3:G40)</f>
+      <c r="L40" s="3"/>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="H41">
+        <f>MIN(G$4:G41)</f>
         <v>72</v>
       </c>
-      <c r="L40" s="3"/>
-    </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="G41">
-        <f>MIN(F$3:F41)</f>
+      <c r="L41" s="3"/>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G42">
+        <f>MIN(F$4:F42)</f>
         <v>51</v>
       </c>
-      <c r="L41" s="3"/>
-    </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F42">
-        <f>MIN(E$3:E42)</f>
+      <c r="L42" s="3"/>
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F43">
+        <f>MIN(E$4:E43)</f>
         <v>24</v>
       </c>
-      <c r="L42" s="3"/>
-    </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="E43">
-        <f>MIN(D$3:D43)</f>
+      <c r="L43" s="3"/>
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="E44">
+        <f>MIN(D$4:D44)</f>
         <v>22</v>
       </c>
-      <c r="L43" s="3"/>
-    </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D44">
-        <f>MIN(C$3:C44)</f>
+      <c r="L44" s="3"/>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D45">
+        <f>MIN(C$4:C45)</f>
         <v>16</v>
       </c>
-      <c r="L44" s="3"/>
-    </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="C45">
-        <f>MIN(B$3:B45)</f>
+      <c r="L45" s="3"/>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C46">
+        <f>MIN(B$4:B46)</f>
         <v>3</v>
       </c>
-      <c r="L45" s="3"/>
-    </row>
-    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B46">
-        <f>L36</f>
+      <c r="L46" s="3"/>
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <f>L37</f>
         <v>1</v>
       </c>
-      <c r="L46" s="4"/>
+      <c r="L47" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>